<commit_message>
11g first version ready
</commit_message>
<xml_diff>
--- a/adm/2019-20/Byrdefordeling19-20.xlsx
+++ b/adm/2019-20/Byrdefordeling19-20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP/adm/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sporring/repositories/PoP/adm/2019-20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{187CBE84-3E2D-F744-A4BD-4B18D538F530}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F14AA-9DBC-854C-BBEE-ECEAD97301D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{C7745739-1061-4147-B11C-6224BC72E703}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Christina</t>
   </si>
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C99A5A-4492-984F-B4EF-E5805ED79020}">
-  <dimension ref="B1:K5"/>
+  <dimension ref="B1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B10" sqref="B10:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,19 +484,19 @@
         <v>16.45</v>
       </c>
       <c r="H2">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="I2" s="2">
         <f>H2/H$5*$F$5</f>
-        <v>178.72340425531914</v>
+        <v>76.595744680851055</v>
       </c>
       <c r="J2" s="2">
         <f>I2+E2</f>
-        <v>178.72340425531914</v>
+        <v>76.595744680851055</v>
       </c>
       <c r="K2" s="1">
         <f>J2/J$5</f>
-        <v>0.25531914893617019</v>
+        <v>0.10942249240121579</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
@@ -557,19 +557,19 @@
         <v>14.1</v>
       </c>
       <c r="H4">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2">
         <f>H4/H$5*$F$5</f>
-        <v>191.48936170212767</v>
+        <v>293.61702127659572</v>
       </c>
       <c r="J4" s="2">
         <f>I4+E4</f>
-        <v>291.48936170212767</v>
+        <v>393.61702127659572</v>
       </c>
       <c r="K4" s="1">
         <f>J4/J$5</f>
-        <v>0.4164133738601824</v>
+        <v>0.56231003039513672</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.2">
@@ -609,7 +609,90 @@
       </c>
       <c r="K5" s="1">
         <f>SUM(K2:K4)</f>
-        <v>1</v>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B11" t="str">
+        <f>B2</f>
+        <v>Christina</v>
+      </c>
+      <c r="C11">
+        <f>H2</f>
+        <v>6</v>
+      </c>
+      <c r="D11" s="2">
+        <f>J2</f>
+        <v>76.595744680851055</v>
+      </c>
+      <c r="E11" s="1">
+        <f>K2</f>
+        <v>0.10942249240121579</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B12" t="str">
+        <f t="shared" ref="B12:B14" si="0">B3</f>
+        <v>Martin</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C14" si="1">H3</f>
+        <v>18</v>
+      </c>
+      <c r="D12" s="2">
+        <f>J3</f>
+        <v>229.78723404255319</v>
+      </c>
+      <c r="E12" s="1">
+        <f>K3</f>
+        <v>0.32826747720364741</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Jon</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D13" s="2">
+        <f>J4</f>
+        <v>393.61702127659572</v>
+      </c>
+      <c r="E13" s="1">
+        <f>K4</f>
+        <v>0.56231003039513672</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Total</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D14" s="2">
+        <f>J5</f>
+        <v>700</v>
+      </c>
+      <c r="E14" s="1">
+        <f>K5</f>
+        <v>0.99999999999999989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>